<commit_message>
files are updated nd about to push at time 2020-10-05 11:06:01
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -708,6 +708,11 @@
           <t>04-10-2020</t>
         </is>
       </c>
+      <c r="T1" s="9" t="inlineStr">
+        <is>
+          <t>05-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -769,6 +774,9 @@
       <c r="S2" t="n">
         <v>173</v>
       </c>
+      <c r="T2" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -830,6 +838,9 @@
       <c r="S3" t="n">
         <v>55282</v>
       </c>
+      <c r="T3" t="n">
+        <v>54400</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -891,6 +902,9 @@
       <c r="S4" t="n">
         <v>3015</v>
       </c>
+      <c r="T4" t="n">
+        <v>2953</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -952,6 +966,9 @@
       <c r="S5" t="n">
         <v>33933</v>
       </c>
+      <c r="T5" t="n">
+        <v>33324</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1013,6 +1030,9 @@
       <c r="S6" t="n">
         <v>11597</v>
       </c>
+      <c r="T6" t="n">
+        <v>11795</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1074,6 +1094,9 @@
       <c r="S7" t="n">
         <v>1792</v>
       </c>
+      <c r="T7" t="n">
+        <v>1673</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1135,6 +1158,9 @@
       <c r="S8" t="n">
         <v>29292</v>
       </c>
+      <c r="T8" t="n">
+        <v>28548</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1196,6 +1222,9 @@
       <c r="S9" t="n">
         <v>101</v>
       </c>
+      <c r="T9" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1257,6 +1286,9 @@
       <c r="S10" t="n">
         <v>25234</v>
       </c>
+      <c r="T10" t="n">
+        <v>24753</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1318,6 +1350,9 @@
       <c r="S11" t="n">
         <v>4923</v>
       </c>
+      <c r="T11" t="n">
+        <v>4839</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1379,6 +1414,9 @@
       <c r="S12" t="n">
         <v>16762</v>
       </c>
+      <c r="T12" t="n">
+        <v>16809</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1440,6 +1478,9 @@
       <c r="S13" t="n">
         <v>12868</v>
       </c>
+      <c r="T13" t="n">
+        <v>12067</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1501,6 +1542,9 @@
       <c r="S14" t="n">
         <v>3292</v>
       </c>
+      <c r="T14" t="n">
+        <v>3273</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1562,6 +1606,9 @@
       <c r="S15" t="n">
         <v>15646</v>
       </c>
+      <c r="T15" t="n">
+        <v>15460</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1623,6 +1670,9 @@
       <c r="S16" t="n">
         <v>10939</v>
       </c>
+      <c r="T16" t="n">
+        <v>10936</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1684,6 +1734,9 @@
       <c r="S17" t="n">
         <v>112802</v>
       </c>
+      <c r="T17" t="n">
+        <v>115593</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1745,6 +1798,9 @@
       <c r="S18" t="n">
         <v>80900</v>
       </c>
+      <c r="T18" t="n">
+        <v>84579</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1806,6 +1862,9 @@
       <c r="S19" t="n">
         <v>1101</v>
       </c>
+      <c r="T19" t="n">
+        <v>1106</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1867,6 +1926,9 @@
       <c r="S20" t="n">
         <v>19807</v>
       </c>
+      <c r="T20" t="n">
+        <v>19372</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1928,6 +1990,9 @@
       <c r="S21" t="n">
         <v>258548</v>
       </c>
+      <c r="T21" t="n">
+        <v>255722</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1989,6 +2054,9 @@
       <c r="S22" t="n">
         <v>2497</v>
       </c>
+      <c r="T22" t="n">
+        <v>2576</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2050,6 +2118,9 @@
       <c r="S23" t="n">
         <v>2083</v>
       </c>
+      <c r="T23" t="n">
+        <v>2209</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2111,6 +2182,9 @@
       <c r="S24" t="n">
         <v>348</v>
       </c>
+      <c r="T24" t="n">
+        <v>313</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2172,6 +2246,9 @@
       <c r="S25" t="n">
         <v>1155</v>
       </c>
+      <c r="T25" t="n">
+        <v>1226</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2233,6 +2310,9 @@
       <c r="S26" t="n">
         <v>30301</v>
       </c>
+      <c r="T26" t="n">
+        <v>29504</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2294,6 +2374,9 @@
       <c r="S27" t="n">
         <v>4874</v>
       </c>
+      <c r="T27" t="n">
+        <v>4787</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2355,6 +2438,9 @@
       <c r="S28" t="n">
         <v>14289</v>
       </c>
+      <c r="T28" t="n">
+        <v>13577</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2416,6 +2502,9 @@
       <c r="S29" t="n">
         <v>21075</v>
       </c>
+      <c r="T29" t="n">
+        <v>21154</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2477,6 +2566,9 @@
       <c r="S30" t="n">
         <v>640</v>
       </c>
+      <c r="T30" t="n">
+        <v>649</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2538,6 +2630,9 @@
       <c r="S31" t="n">
         <v>46255</v>
       </c>
+      <c r="T31" t="n">
+        <v>46120</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2599,6 +2694,9 @@
       <c r="S32" t="n">
         <v>27901</v>
       </c>
+      <c r="T32" t="n">
+        <v>27052</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2660,6 +2758,9 @@
       <c r="S33" t="n">
         <v>5171</v>
       </c>
+      <c r="T33" t="n">
+        <v>4858</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2721,6 +2822,9 @@
       <c r="S34" t="n">
         <v>8076</v>
       </c>
+      <c r="T34" t="n">
+        <v>9089</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2782,6 +2886,9 @@
       <c r="S35" t="n">
         <v>47823</v>
       </c>
+      <c r="T35" t="n">
+        <v>46385</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2842,6 +2949,9 @@
       </c>
       <c r="S36" t="n">
         <v>27130</v>
+      </c>
+      <c r="T36" t="n">
+        <v>27439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-06 10:37:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -713,6 +713,11 @@
           <t>05-10-2020</t>
         </is>
       </c>
+      <c r="U1" s="9" t="inlineStr">
+        <is>
+          <t>06-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -777,6 +782,9 @@
       <c r="T2" t="n">
         <v>182</v>
       </c>
+      <c r="U2" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -841,6 +849,9 @@
       <c r="T3" t="n">
         <v>54400</v>
       </c>
+      <c r="U3" t="n">
+        <v>51060</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -905,6 +916,9 @@
       <c r="T4" t="n">
         <v>2953</v>
       </c>
+      <c r="U4" t="n">
+        <v>2989</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -969,6 +983,9 @@
       <c r="T5" t="n">
         <v>33324</v>
       </c>
+      <c r="U5" t="n">
+        <v>33467</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1033,6 +1050,9 @@
       <c r="T6" t="n">
         <v>11795</v>
       </c>
+      <c r="U6" t="n">
+        <v>11523</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1097,6 +1117,9 @@
       <c r="T7" t="n">
         <v>1673</v>
       </c>
+      <c r="U7" t="n">
+        <v>1604</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1161,6 +1184,9 @@
       <c r="T8" t="n">
         <v>28548</v>
       </c>
+      <c r="U8" t="n">
+        <v>27857</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1225,6 +1251,9 @@
       <c r="T9" t="n">
         <v>105</v>
       </c>
+      <c r="U9" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1289,6 +1318,9 @@
       <c r="T10" t="n">
         <v>24753</v>
       </c>
+      <c r="U10" t="n">
+        <v>23080</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1353,6 +1385,9 @@
       <c r="T11" t="n">
         <v>4839</v>
       </c>
+      <c r="U11" t="n">
+        <v>4803</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1417,6 +1452,9 @@
       <c r="T12" t="n">
         <v>16809</v>
       </c>
+      <c r="U12" t="n">
+        <v>16718</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1481,6 +1519,9 @@
       <c r="T13" t="n">
         <v>12067</v>
       </c>
+      <c r="U13" t="n">
+        <v>11822</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1545,6 +1586,9 @@
       <c r="T14" t="n">
         <v>3273</v>
       </c>
+      <c r="U14" t="n">
+        <v>3156</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1609,6 +1653,9 @@
       <c r="T15" t="n">
         <v>15460</v>
       </c>
+      <c r="U15" t="n">
+        <v>14696</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1673,6 +1720,9 @@
       <c r="T16" t="n">
         <v>10936</v>
       </c>
+      <c r="U16" t="n">
+        <v>10436</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1737,6 +1787,9 @@
       <c r="T17" t="n">
         <v>115593</v>
       </c>
+      <c r="U17" t="n">
+        <v>115496</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1801,6 +1854,9 @@
       <c r="T18" t="n">
         <v>84579</v>
       </c>
+      <c r="U18" t="n">
+        <v>84958</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1865,6 +1921,9 @@
       <c r="T19" t="n">
         <v>1106</v>
       </c>
+      <c r="U19" t="n">
+        <v>1166</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1929,6 +1988,9 @@
       <c r="T20" t="n">
         <v>19372</v>
       </c>
+      <c r="U20" t="n">
+        <v>18757</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1993,6 +2055,9 @@
       <c r="T21" t="n">
         <v>255722</v>
       </c>
+      <c r="U21" t="n">
+        <v>252721</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2057,6 +2122,9 @@
       <c r="T22" t="n">
         <v>2576</v>
       </c>
+      <c r="U22" t="n">
+        <v>2696</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2121,6 +2189,9 @@
       <c r="T23" t="n">
         <v>2209</v>
       </c>
+      <c r="U23" t="n">
+        <v>2217</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2185,6 +2256,9 @@
       <c r="T24" t="n">
         <v>313</v>
       </c>
+      <c r="U24" t="n">
+        <v>291</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2249,6 +2323,9 @@
       <c r="T25" t="n">
         <v>1226</v>
       </c>
+      <c r="U25" t="n">
+        <v>1155</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2313,6 +2390,9 @@
       <c r="T26" t="n">
         <v>29504</v>
       </c>
+      <c r="U26" t="n">
+        <v>28006</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2377,6 +2457,9 @@
       <c r="T27" t="n">
         <v>4787</v>
       </c>
+      <c r="U27" t="n">
+        <v>4513</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2441,6 +2524,9 @@
       <c r="T28" t="n">
         <v>13577</v>
       </c>
+      <c r="U28" t="n">
+        <v>12895</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2505,6 +2591,9 @@
       <c r="T29" t="n">
         <v>21154</v>
       </c>
+      <c r="U29" t="n">
+        <v>21215</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2569,6 +2658,9 @@
       <c r="T30" t="n">
         <v>649</v>
       </c>
+      <c r="U30" t="n">
+        <v>598</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2633,6 +2725,9 @@
       <c r="T31" t="n">
         <v>46120</v>
       </c>
+      <c r="U31" t="n">
+        <v>45881</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2697,6 +2792,9 @@
       <c r="T32" t="n">
         <v>27052</v>
       </c>
+      <c r="U32" t="n">
+        <v>26644</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2761,6 +2859,9 @@
       <c r="T33" t="n">
         <v>4858</v>
       </c>
+      <c r="U33" t="n">
+        <v>4876</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2825,6 +2926,9 @@
       <c r="T34" t="n">
         <v>9089</v>
       </c>
+      <c r="U34" t="n">
+        <v>8701</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2889,6 +2993,9 @@
       <c r="T35" t="n">
         <v>46385</v>
       </c>
+      <c r="U35" t="n">
+        <v>45024</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2952,6 +3059,9 @@
       </c>
       <c r="T36" t="n">
         <v>27439</v>
+      </c>
+      <c r="U36" t="n">
+        <v>27717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-07 10:37:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -718,6 +718,11 @@
           <t>06-10-2020</t>
         </is>
       </c>
+      <c r="V1" s="9" t="inlineStr">
+        <is>
+          <t>07-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -785,6 +790,9 @@
       <c r="U2" t="n">
         <v>186</v>
       </c>
+      <c r="V2" t="n">
+        <v>180</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -852,6 +860,9 @@
       <c r="U3" t="n">
         <v>51060</v>
       </c>
+      <c r="V3" t="n">
+        <v>50776</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -919,6 +930,9 @@
       <c r="U4" t="n">
         <v>2989</v>
       </c>
+      <c r="V4" t="n">
+        <v>3022</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -986,6 +1000,9 @@
       <c r="U5" t="n">
         <v>33467</v>
       </c>
+      <c r="V5" t="n">
+        <v>33047</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1053,6 +1070,9 @@
       <c r="U6" t="n">
         <v>11523</v>
       </c>
+      <c r="V6" t="n">
+        <v>11420</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1120,6 +1140,9 @@
       <c r="U7" t="n">
         <v>1604</v>
       </c>
+      <c r="V7" t="n">
+        <v>1492</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1187,6 +1210,9 @@
       <c r="U8" t="n">
         <v>27857</v>
       </c>
+      <c r="V8" t="n">
+        <v>27238</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1254,6 +1280,9 @@
       <c r="U9" t="n">
         <v>99</v>
       </c>
+      <c r="V9" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1321,6 +1350,9 @@
       <c r="U10" t="n">
         <v>23080</v>
       </c>
+      <c r="V10" t="n">
+        <v>22720</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1388,6 +1420,9 @@
       <c r="U11" t="n">
         <v>4803</v>
       </c>
+      <c r="V11" t="n">
+        <v>4720</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1455,6 +1490,9 @@
       <c r="U12" t="n">
         <v>16718</v>
       </c>
+      <c r="V12" t="n">
+        <v>16570</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1522,6 +1560,9 @@
       <c r="U13" t="n">
         <v>11822</v>
       </c>
+      <c r="V13" t="n">
+        <v>11320</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1589,6 +1630,9 @@
       <c r="U14" t="n">
         <v>3156</v>
       </c>
+      <c r="V14" t="n">
+        <v>3136</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1656,6 +1700,9 @@
       <c r="U15" t="n">
         <v>14696</v>
       </c>
+      <c r="V15" t="n">
+        <v>13712</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1723,6 +1770,9 @@
       <c r="U16" t="n">
         <v>10436</v>
       </c>
+      <c r="V16" t="n">
+        <v>10027</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1790,6 +1840,9 @@
       <c r="U17" t="n">
         <v>115496</v>
       </c>
+      <c r="V17" t="n">
+        <v>115170</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1857,6 +1910,9 @@
       <c r="U18" t="n">
         <v>84958</v>
       </c>
+      <c r="V18" t="n">
+        <v>87823</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1924,6 +1980,9 @@
       <c r="U19" t="n">
         <v>1166</v>
       </c>
+      <c r="V19" t="n">
+        <v>1195</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1991,6 +2050,9 @@
       <c r="U20" t="n">
         <v>18757</v>
       </c>
+      <c r="V20" t="n">
+        <v>18141</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2058,6 +2120,9 @@
       <c r="U21" t="n">
         <v>252721</v>
       </c>
+      <c r="V21" t="n">
+        <v>247468</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2125,6 +2190,9 @@
       <c r="U22" t="n">
         <v>2696</v>
       </c>
+      <c r="V22" t="n">
+        <v>2680</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2192,6 +2260,9 @@
       <c r="U23" t="n">
         <v>2217</v>
       </c>
+      <c r="V23" t="n">
+        <v>2371</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2259,6 +2330,9 @@
       <c r="U24" t="n">
         <v>291</v>
       </c>
+      <c r="V24" t="n">
+        <v>261</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2326,6 +2400,9 @@
       <c r="U25" t="n">
         <v>1155</v>
       </c>
+      <c r="V25" t="n">
+        <v>1185</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2393,6 +2470,9 @@
       <c r="U26" t="n">
         <v>28006</v>
       </c>
+      <c r="V26" t="n">
+        <v>26846</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2460,6 +2540,9 @@
       <c r="U27" t="n">
         <v>4513</v>
       </c>
+      <c r="V27" t="n">
+        <v>4522</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2527,6 +2610,9 @@
       <c r="U28" t="n">
         <v>12895</v>
       </c>
+      <c r="V28" t="n">
+        <v>11982</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2594,6 +2680,9 @@
       <c r="U29" t="n">
         <v>21215</v>
       </c>
+      <c r="V29" t="n">
+        <v>21294</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2661,6 +2750,9 @@
       <c r="U30" t="n">
         <v>598</v>
       </c>
+      <c r="V30" t="n">
+        <v>580</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2728,6 +2820,9 @@
       <c r="U31" t="n">
         <v>45881</v>
       </c>
+      <c r="V31" t="n">
+        <v>45279</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2795,6 +2890,9 @@
       <c r="U32" t="n">
         <v>26644</v>
       </c>
+      <c r="V32" t="n">
+        <v>26551</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2862,6 +2960,9 @@
       <c r="U33" t="n">
         <v>4876</v>
       </c>
+      <c r="V33" t="n">
+        <v>4621</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2929,6 +3030,9 @@
       <c r="U34" t="n">
         <v>8701</v>
       </c>
+      <c r="V34" t="n">
+        <v>8414</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2996,6 +3100,9 @@
       <c r="U35" t="n">
         <v>45024</v>
       </c>
+      <c r="V35" t="n">
+        <v>44031</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3062,6 +3169,9 @@
       </c>
       <c r="U36" t="n">
         <v>27717</v>
+      </c>
+      <c r="V36" t="n">
+        <v>27988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-08 10:37:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -723,6 +723,11 @@
           <t>07-10-2020</t>
         </is>
       </c>
+      <c r="W1" s="9" t="inlineStr">
+        <is>
+          <t>08-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -793,6 +798,9 @@
       <c r="V2" t="n">
         <v>180</v>
       </c>
+      <c r="W2" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -863,6 +871,9 @@
       <c r="V3" t="n">
         <v>50776</v>
       </c>
+      <c r="W3" t="n">
+        <v>49513</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -933,6 +944,9 @@
       <c r="V4" t="n">
         <v>3022</v>
       </c>
+      <c r="W4" t="n">
+        <v>2850</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1003,6 +1017,9 @@
       <c r="V5" t="n">
         <v>33047</v>
       </c>
+      <c r="W5" t="n">
+        <v>31786</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1073,6 +1090,9 @@
       <c r="V6" t="n">
         <v>11420</v>
       </c>
+      <c r="W6" t="n">
+        <v>11326</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1143,6 +1163,9 @@
       <c r="V7" t="n">
         <v>1492</v>
       </c>
+      <c r="W7" t="n">
+        <v>1448</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1213,6 +1236,9 @@
       <c r="V8" t="n">
         <v>27238</v>
       </c>
+      <c r="W8" t="n">
+        <v>26777</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1283,6 +1309,9 @@
       <c r="V9" t="n">
         <v>101</v>
       </c>
+      <c r="W9" t="n">
+        <v>108</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1353,6 +1382,9 @@
       <c r="V10" t="n">
         <v>22720</v>
       </c>
+      <c r="W10" t="n">
+        <v>22186</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1423,6 +1455,9 @@
       <c r="V11" t="n">
         <v>4720</v>
       </c>
+      <c r="W11" t="n">
+        <v>4749</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1493,6 +1528,9 @@
       <c r="V12" t="n">
         <v>16570</v>
       </c>
+      <c r="W12" t="n">
+        <v>16485</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1563,6 +1601,9 @@
       <c r="V13" t="n">
         <v>11320</v>
       </c>
+      <c r="W13" t="n">
+        <v>11029</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1633,6 +1674,9 @@
       <c r="V14" t="n">
         <v>3136</v>
       </c>
+      <c r="W14" t="n">
+        <v>2996</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1703,6 +1747,9 @@
       <c r="V15" t="n">
         <v>13712</v>
       </c>
+      <c r="W15" t="n">
+        <v>12131</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1773,6 +1820,9 @@
       <c r="V16" t="n">
         <v>10027</v>
       </c>
+      <c r="W16" t="n">
+        <v>9759</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1843,6 +1893,9 @@
       <c r="V17" t="n">
         <v>115170</v>
       </c>
+      <c r="W17" t="n">
+        <v>116172</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1913,6 +1966,9 @@
       <c r="V18" t="n">
         <v>87823</v>
       </c>
+      <c r="W18" t="n">
+        <v>92246</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1983,6 +2039,9 @@
       <c r="V19" t="n">
         <v>1195</v>
       </c>
+      <c r="W19" t="n">
+        <v>1228</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2053,6 +2112,9 @@
       <c r="V20" t="n">
         <v>18141</v>
       </c>
+      <c r="W20" t="n">
+        <v>17522</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2123,6 +2185,9 @@
       <c r="V21" t="n">
         <v>247468</v>
       </c>
+      <c r="W21" t="n">
+        <v>244976</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2193,6 +2258,9 @@
       <c r="V22" t="n">
         <v>2680</v>
       </c>
+      <c r="W22" t="n">
+        <v>2805</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2263,6 +2331,9 @@
       <c r="V23" t="n">
         <v>2371</v>
       </c>
+      <c r="W23" t="n">
+        <v>2411</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2333,6 +2404,9 @@
       <c r="V24" t="n">
         <v>261</v>
       </c>
+      <c r="W24" t="n">
+        <v>231</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2403,6 +2477,9 @@
       <c r="V25" t="n">
         <v>1185</v>
       </c>
+      <c r="W25" t="n">
+        <v>1200</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2473,6 +2550,9 @@
       <c r="V26" t="n">
         <v>26846</v>
       </c>
+      <c r="W26" t="n">
+        <v>26368</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2543,6 +2623,9 @@
       <c r="V27" t="n">
         <v>4522</v>
       </c>
+      <c r="W27" t="n">
+        <v>4680</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2613,6 +2696,9 @@
       <c r="V28" t="n">
         <v>11982</v>
       </c>
+      <c r="W28" t="n">
+        <v>11563</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2683,6 +2769,9 @@
       <c r="V29" t="n">
         <v>21294</v>
       </c>
+      <c r="W29" t="n">
+        <v>21351</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2753,6 +2842,9 @@
       <c r="V30" t="n">
         <v>580</v>
       </c>
+      <c r="W30" t="n">
+        <v>570</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2823,6 +2915,9 @@
       <c r="V31" t="n">
         <v>45279</v>
       </c>
+      <c r="W31" t="n">
+        <v>45135</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2893,6 +2988,9 @@
       <c r="V32" t="n">
         <v>26551</v>
       </c>
+      <c r="W32" t="n">
+        <v>26368</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2963,6 +3061,9 @@
       <c r="V33" t="n">
         <v>4621</v>
       </c>
+      <c r="W33" t="n">
+        <v>4389</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3033,6 +3134,9 @@
       <c r="V34" t="n">
         <v>8414</v>
       </c>
+      <c r="W34" t="n">
+        <v>8367</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3103,6 +3207,9 @@
       <c r="V35" t="n">
         <v>44031</v>
       </c>
+      <c r="W35" t="n">
+        <v>43154</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3172,6 +3279,9 @@
       </c>
       <c r="V36" t="n">
         <v>27988</v>
+      </c>
+      <c r="W36" t="n">
+        <v>28361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-09 10:37:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -728,6 +728,11 @@
           <t>08-10-2020</t>
         </is>
       </c>
+      <c r="X1" s="9" t="inlineStr">
+        <is>
+          <t>09-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -801,6 +806,9 @@
       <c r="W2" t="n">
         <v>185</v>
       </c>
+      <c r="X2" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -874,6 +882,9 @@
       <c r="W3" t="n">
         <v>49513</v>
       </c>
+      <c r="X3" t="n">
+        <v>48661</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -947,6 +958,9 @@
       <c r="W4" t="n">
         <v>2850</v>
       </c>
+      <c r="X4" t="n">
+        <v>2778</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1020,6 +1034,9 @@
       <c r="W5" t="n">
         <v>31786</v>
       </c>
+      <c r="X5" t="n">
+        <v>30767</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1093,6 +1110,9 @@
       <c r="W6" t="n">
         <v>11326</v>
       </c>
+      <c r="X6" t="n">
+        <v>11447</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1166,6 +1186,9 @@
       <c r="W7" t="n">
         <v>1448</v>
       </c>
+      <c r="X7" t="n">
+        <v>1392</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1239,6 +1262,9 @@
       <c r="W8" t="n">
         <v>26777</v>
       </c>
+      <c r="X8" t="n">
+        <v>27427</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1312,6 +1338,9 @@
       <c r="W9" t="n">
         <v>108</v>
       </c>
+      <c r="X9" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1385,6 +1414,9 @@
       <c r="W10" t="n">
         <v>22186</v>
       </c>
+      <c r="X10" t="n">
+        <v>22232</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1458,6 +1490,9 @@
       <c r="W11" t="n">
         <v>4749</v>
       </c>
+      <c r="X11" t="n">
+        <v>4716</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1531,6 +1566,9 @@
       <c r="W12" t="n">
         <v>16485</v>
       </c>
+      <c r="X12" t="n">
+        <v>16465</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1604,6 +1642,9 @@
       <c r="W13" t="n">
         <v>11029</v>
       </c>
+      <c r="X13" t="n">
+        <v>10867</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1677,6 +1718,9 @@
       <c r="W14" t="n">
         <v>2996</v>
       </c>
+      <c r="X14" t="n">
+        <v>2943</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1750,6 +1794,9 @@
       <c r="W15" t="n">
         <v>12131</v>
       </c>
+      <c r="X15" t="n">
+        <v>11482</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1823,6 +1870,9 @@
       <c r="W16" t="n">
         <v>9759</v>
       </c>
+      <c r="X16" t="n">
+        <v>9272</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1896,6 +1946,9 @@
       <c r="W17" t="n">
         <v>116172</v>
       </c>
+      <c r="X17" t="n">
+        <v>117162</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1969,6 +2022,9 @@
       <c r="W18" t="n">
         <v>92246</v>
       </c>
+      <c r="X18" t="n">
+        <v>90664</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2042,6 +2098,9 @@
       <c r="W19" t="n">
         <v>1228</v>
       </c>
+      <c r="X19" t="n">
+        <v>1299</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2115,6 +2174,9 @@
       <c r="W20" t="n">
         <v>17522</v>
       </c>
+      <c r="X20" t="n">
+        <v>16788</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2188,6 +2250,9 @@
       <c r="W21" t="n">
         <v>244976</v>
       </c>
+      <c r="X21" t="n">
+        <v>242438</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2261,6 +2326,9 @@
       <c r="W22" t="n">
         <v>2805</v>
       </c>
+      <c r="X22" t="n">
+        <v>2877</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2334,6 +2402,9 @@
       <c r="W23" t="n">
         <v>2411</v>
       </c>
+      <c r="X23" t="n">
+        <v>2369</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2407,6 +2478,9 @@
       <c r="W24" t="n">
         <v>231</v>
       </c>
+      <c r="X24" t="n">
+        <v>220</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2480,6 +2554,9 @@
       <c r="W25" t="n">
         <v>1200</v>
       </c>
+      <c r="X25" t="n">
+        <v>1155</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2553,6 +2630,9 @@
       <c r="W26" t="n">
         <v>26368</v>
       </c>
+      <c r="X26" t="n">
+        <v>26184</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2626,6 +2706,9 @@
       <c r="W27" t="n">
         <v>4680</v>
       </c>
+      <c r="X27" t="n">
+        <v>4727</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2699,6 +2782,9 @@
       <c r="W28" t="n">
         <v>11563</v>
       </c>
+      <c r="X28" t="n">
+        <v>10775</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2772,6 +2858,9 @@
       <c r="W29" t="n">
         <v>21351</v>
       </c>
+      <c r="X29" t="n">
+        <v>21382</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2845,6 +2934,9 @@
       <c r="W30" t="n">
         <v>570</v>
       </c>
+      <c r="X30" t="n">
+        <v>545</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2918,6 +3010,9 @@
       <c r="W31" t="n">
         <v>45135</v>
       </c>
+      <c r="X31" t="n">
+        <v>44437</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2991,6 +3086,9 @@
       <c r="W32" t="n">
         <v>26368</v>
       </c>
+      <c r="X32" t="n">
+        <v>26374</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3064,6 +3162,9 @@
       <c r="W33" t="n">
         <v>4389</v>
       </c>
+      <c r="X33" t="n">
+        <v>4197</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3137,6 +3238,9 @@
       <c r="W34" t="n">
         <v>8367</v>
       </c>
+      <c r="X34" t="n">
+        <v>7849</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3210,6 +3314,9 @@
       <c r="W35" t="n">
         <v>43154</v>
       </c>
+      <c r="X35" t="n">
+        <v>42552</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3282,6 +3389,9 @@
       </c>
       <c r="W36" t="n">
         <v>28361</v>
+      </c>
+      <c r="X36" t="n">
+        <v>28854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-10 10:35:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -733,6 +733,11 @@
           <t>09-10-2020</t>
         </is>
       </c>
+      <c r="Y1" s="9" t="inlineStr">
+        <is>
+          <t>10-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -809,6 +814,9 @@
       <c r="X2" t="n">
         <v>190</v>
       </c>
+      <c r="Y2" t="n">
+        <v>197</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -885,6 +893,9 @@
       <c r="X3" t="n">
         <v>48661</v>
       </c>
+      <c r="Y3" t="n">
+        <v>47665</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -961,6 +972,9 @@
       <c r="X4" t="n">
         <v>2778</v>
       </c>
+      <c r="Y4" t="n">
+        <v>2860</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1037,6 +1051,9 @@
       <c r="X5" t="n">
         <v>30767</v>
       </c>
+      <c r="Y5" t="n">
+        <v>29710</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1113,6 +1130,9 @@
       <c r="X6" t="n">
         <v>11447</v>
       </c>
+      <c r="Y6" t="n">
+        <v>11274</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1189,6 +1209,9 @@
       <c r="X7" t="n">
         <v>1392</v>
       </c>
+      <c r="Y7" t="n">
+        <v>1292</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1265,6 +1288,9 @@
       <c r="X8" t="n">
         <v>27427</v>
       </c>
+      <c r="Y8" t="n">
+        <v>27439</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1341,6 +1367,9 @@
       <c r="X9" t="n">
         <v>105</v>
       </c>
+      <c r="Y9" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1417,6 +1446,9 @@
       <c r="X10" t="n">
         <v>22232</v>
       </c>
+      <c r="Y10" t="n">
+        <v>21955</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1493,6 +1525,9 @@
       <c r="X11" t="n">
         <v>4716</v>
       </c>
+      <c r="Y11" t="n">
+        <v>4783</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1569,6 +1604,9 @@
       <c r="X12" t="n">
         <v>16465</v>
       </c>
+      <c r="Y12" t="n">
+        <v>16181</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1645,6 +1683,9 @@
       <c r="X13" t="n">
         <v>10867</v>
       </c>
+      <c r="Y13" t="n">
+        <v>10830</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1721,6 +1762,9 @@
       <c r="X14" t="n">
         <v>2943</v>
       </c>
+      <c r="Y14" t="n">
+        <v>2856</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1797,6 +1841,9 @@
       <c r="X15" t="n">
         <v>11482</v>
       </c>
+      <c r="Y15" t="n">
+        <v>11144</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1873,6 +1920,9 @@
       <c r="X16" t="n">
         <v>9272</v>
       </c>
+      <c r="Y16" t="n">
+        <v>8819</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1949,6 +1999,9 @@
       <c r="X17" t="n">
         <v>117162</v>
       </c>
+      <c r="Y17" t="n">
+        <v>118870</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2025,6 +2078,9 @@
       <c r="X18" t="n">
         <v>90664</v>
       </c>
+      <c r="Y18" t="n">
+        <v>91841</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2101,6 +2157,9 @@
       <c r="X19" t="n">
         <v>1299</v>
       </c>
+      <c r="Y19" t="n">
+        <v>1038</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2177,6 +2236,9 @@
       <c r="X20" t="n">
         <v>16788</v>
       </c>
+      <c r="Y20" t="n">
+        <v>16168</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2253,6 +2315,9 @@
       <c r="X21" t="n">
         <v>242438</v>
       </c>
+      <c r="Y21" t="n">
+        <v>236947</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2329,6 +2394,9 @@
       <c r="X22" t="n">
         <v>2877</v>
       </c>
+      <c r="Y22" t="n">
+        <v>2858</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2405,6 +2473,9 @@
       <c r="X23" t="n">
         <v>2369</v>
       </c>
+      <c r="Y23" t="n">
+        <v>2424</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2481,6 +2552,9 @@
       <c r="X24" t="n">
         <v>220</v>
       </c>
+      <c r="Y24" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2557,6 +2631,9 @@
       <c r="X25" t="n">
         <v>1155</v>
       </c>
+      <c r="Y25" t="n">
+        <v>1215</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2633,6 +2710,9 @@
       <c r="X26" t="n">
         <v>26184</v>
       </c>
+      <c r="Y26" t="n">
+        <v>25460</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2709,6 +2789,9 @@
       <c r="X27" t="n">
         <v>4727</v>
       </c>
+      <c r="Y27" t="n">
+        <v>4803</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2785,6 +2868,9 @@
       <c r="X28" t="n">
         <v>10775</v>
       </c>
+      <c r="Y28" t="n">
+        <v>10153</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2861,6 +2947,9 @@
       <c r="X29" t="n">
         <v>21382</v>
       </c>
+      <c r="Y29" t="n">
+        <v>21398</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2937,6 +3026,9 @@
       <c r="X30" t="n">
         <v>545</v>
       </c>
+      <c r="Y30" t="n">
+        <v>504</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3013,6 +3105,9 @@
       <c r="X31" t="n">
         <v>44437</v>
       </c>
+      <c r="Y31" t="n">
+        <v>44197</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3089,6 +3184,9 @@
       <c r="X32" t="n">
         <v>26374</v>
       </c>
+      <c r="Y32" t="n">
+        <v>26104</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3165,6 +3263,9 @@
       <c r="X33" t="n">
         <v>4197</v>
       </c>
+      <c r="Y33" t="n">
+        <v>4039</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3241,6 +3342,9 @@
       <c r="X34" t="n">
         <v>7849</v>
       </c>
+      <c r="Y34" t="n">
+        <v>7289</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3317,6 +3421,9 @@
       <c r="X35" t="n">
         <v>42552</v>
       </c>
+      <c r="Y35" t="n">
+        <v>41287</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3392,6 +3499,9 @@
       </c>
       <c r="X36" t="n">
         <v>28854</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>29296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-11 10:35:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y36"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -738,6 +738,11 @@
           <t>10-10-2020</t>
         </is>
       </c>
+      <c r="Z1" s="9" t="inlineStr">
+        <is>
+          <t>11-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -817,6 +822,9 @@
       <c r="Y2" t="n">
         <v>197</v>
       </c>
+      <c r="Z2" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -896,6 +904,9 @@
       <c r="Y3" t="n">
         <v>47665</v>
       </c>
+      <c r="Z3" t="n">
+        <v>46624</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -975,6 +986,9 @@
       <c r="Y4" t="n">
         <v>2860</v>
       </c>
+      <c r="Z4" t="n">
+        <v>2940</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1054,6 +1068,9 @@
       <c r="Y5" t="n">
         <v>29710</v>
       </c>
+      <c r="Z5" t="n">
+        <v>29221</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1133,6 +1150,9 @@
       <c r="Y6" t="n">
         <v>11274</v>
       </c>
+      <c r="Z6" t="n">
+        <v>11165</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1212,6 +1232,9 @@
       <c r="Y7" t="n">
         <v>1292</v>
       </c>
+      <c r="Z7" t="n">
+        <v>1229</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1291,6 +1314,9 @@
       <c r="Y8" t="n">
         <v>27439</v>
       </c>
+      <c r="Z8" t="n">
+        <v>27369</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1370,6 +1396,9 @@
       <c r="Y9" t="n">
         <v>101</v>
       </c>
+      <c r="Z9" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1449,6 +1478,9 @@
       <c r="Y10" t="n">
         <v>21955</v>
       </c>
+      <c r="Z10" t="n">
+        <v>22007</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1528,6 +1560,9 @@
       <c r="Y11" t="n">
         <v>4783</v>
       </c>
+      <c r="Z11" t="n">
+        <v>4658</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1607,6 +1642,9 @@
       <c r="Y12" t="n">
         <v>16181</v>
       </c>
+      <c r="Z12" t="n">
+        <v>15936</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1686,6 +1724,9 @@
       <c r="Y13" t="n">
         <v>10830</v>
       </c>
+      <c r="Z13" t="n">
+        <v>10677</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1765,6 +1806,9 @@
       <c r="Y14" t="n">
         <v>2856</v>
       </c>
+      <c r="Z14" t="n">
+        <v>2718</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1844,6 +1888,9 @@
       <c r="Y15" t="n">
         <v>11144</v>
       </c>
+      <c r="Z15" t="n">
+        <v>10796</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1923,6 +1970,9 @@
       <c r="Y16" t="n">
         <v>8819</v>
       </c>
+      <c r="Z16" t="n">
+        <v>8362</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2002,6 +2052,9 @@
       <c r="Y17" t="n">
         <v>118870</v>
       </c>
+      <c r="Z17" t="n">
+        <v>120948</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2081,6 +2134,9 @@
       <c r="Y18" t="n">
         <v>91841</v>
       </c>
+      <c r="Z18" t="n">
+        <v>96003</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2160,6 +2216,9 @@
       <c r="Y19" t="n">
         <v>1038</v>
       </c>
+      <c r="Z19" t="n">
+        <v>1022</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2239,6 +2298,9 @@
       <c r="Y20" t="n">
         <v>16168</v>
       </c>
+      <c r="Z20" t="n">
+        <v>15612</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2318,6 +2380,9 @@
       <c r="Y21" t="n">
         <v>236947</v>
       </c>
+      <c r="Z21" t="n">
+        <v>221615</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2397,6 +2462,9 @@
       <c r="Y22" t="n">
         <v>2858</v>
       </c>
+      <c r="Z22" t="n">
+        <v>2608</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2476,6 +2544,9 @@
       <c r="Y23" t="n">
         <v>2424</v>
       </c>
+      <c r="Z23" t="n">
+        <v>2437</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2555,6 +2626,9 @@
       <c r="Y24" t="n">
         <v>188</v>
       </c>
+      <c r="Z24" t="n">
+        <v>191</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2634,6 +2708,9 @@
       <c r="Y25" t="n">
         <v>1215</v>
       </c>
+      <c r="Z25" t="n">
+        <v>1238</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2713,6 +2790,9 @@
       <c r="Y26" t="n">
         <v>25460</v>
       </c>
+      <c r="Z26" t="n">
+        <v>24414</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2792,6 +2872,9 @@
       <c r="Y27" t="n">
         <v>4803</v>
       </c>
+      <c r="Z27" t="n">
+        <v>4719</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2871,6 +2954,9 @@
       <c r="Y28" t="n">
         <v>10153</v>
       </c>
+      <c r="Z28" t="n">
+        <v>9752</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2950,6 +3036,9 @@
       <c r="Y29" t="n">
         <v>21398</v>
       </c>
+      <c r="Z29" t="n">
+        <v>21354</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3029,6 +3118,9 @@
       <c r="Y30" t="n">
         <v>504</v>
       </c>
+      <c r="Z30" t="n">
+        <v>450</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3108,6 +3200,9 @@
       <c r="Y31" t="n">
         <v>44197</v>
       </c>
+      <c r="Z31" t="n">
+        <v>44150</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3187,6 +3282,9 @@
       <c r="Y32" t="n">
         <v>26104</v>
       </c>
+      <c r="Z32" t="n">
+        <v>25713</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3266,6 +3364,9 @@
       <c r="Y33" t="n">
         <v>4039</v>
       </c>
+      <c r="Z33" t="n">
+        <v>3951</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3345,6 +3446,9 @@
       <c r="Y34" t="n">
         <v>7289</v>
       </c>
+      <c r="Z34" t="n">
+        <v>7321</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3424,6 +3528,9 @@
       <c r="Y35" t="n">
         <v>41287</v>
       </c>
+      <c r="Z35" t="n">
+        <v>40210</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3502,6 +3609,9 @@
       </c>
       <c r="Y36" t="n">
         <v>29296</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>29793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-12 10:35:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -743,6 +743,11 @@
           <t>11-10-2020</t>
         </is>
       </c>
+      <c r="AA1" s="9" t="inlineStr">
+        <is>
+          <t>12-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -825,6 +830,9 @@
       <c r="Z2" t="n">
         <v>193</v>
       </c>
+      <c r="AA2" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -907,6 +915,9 @@
       <c r="Z3" t="n">
         <v>46624</v>
       </c>
+      <c r="AA3" t="n">
+        <v>46295</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -989,6 +1000,9 @@
       <c r="Z4" t="n">
         <v>2940</v>
       </c>
+      <c r="AA4" t="n">
+        <v>2891</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1071,6 +1085,9 @@
       <c r="Z5" t="n">
         <v>29221</v>
       </c>
+      <c r="AA5" t="n">
+        <v>28385</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1153,6 +1170,9 @@
       <c r="Z6" t="n">
         <v>11165</v>
       </c>
+      <c r="AA6" t="n">
+        <v>11044</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1235,6 +1255,9 @@
       <c r="Z7" t="n">
         <v>1229</v>
       </c>
+      <c r="AA7" t="n">
+        <v>1184</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1317,6 +1340,9 @@
       <c r="Z8" t="n">
         <v>27369</v>
       </c>
+      <c r="AA8" t="n">
+        <v>27348</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1399,6 +1425,9 @@
       <c r="Z9" t="n">
         <v>100</v>
       </c>
+      <c r="AA9" t="n">
+        <v>102</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1481,6 +1510,9 @@
       <c r="Z10" t="n">
         <v>22007</v>
       </c>
+      <c r="AA10" t="n">
+        <v>21701</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1563,6 +1595,9 @@
       <c r="Z11" t="n">
         <v>4658</v>
       </c>
+      <c r="AA11" t="n">
+        <v>4656</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1645,6 +1680,9 @@
       <c r="Z12" t="n">
         <v>15936</v>
       </c>
+      <c r="AA12" t="n">
+        <v>15695</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1727,6 +1765,9 @@
       <c r="Z13" t="n">
         <v>10677</v>
       </c>
+      <c r="AA13" t="n">
+        <v>10573</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1809,6 +1850,9 @@
       <c r="Z14" t="n">
         <v>2718</v>
       </c>
+      <c r="AA14" t="n">
+        <v>2687</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1891,6 +1935,9 @@
       <c r="Z15" t="n">
         <v>10796</v>
       </c>
+      <c r="AA15" t="n">
+        <v>10466</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1973,6 +2020,9 @@
       <c r="Z16" t="n">
         <v>8362</v>
       </c>
+      <c r="AA16" t="n">
+        <v>8167</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2055,6 +2105,9 @@
       <c r="Z17" t="n">
         <v>120948</v>
       </c>
+      <c r="AA17" t="n">
+        <v>120289</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2137,6 +2190,9 @@
       <c r="Z18" t="n">
         <v>96003</v>
       </c>
+      <c r="AA18" t="n">
+        <v>96401</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2219,6 +2275,9 @@
       <c r="Z19" t="n">
         <v>1022</v>
       </c>
+      <c r="AA19" t="n">
+        <v>980</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2301,6 +2360,9 @@
       <c r="Z20" t="n">
         <v>15612</v>
       </c>
+      <c r="AA20" t="n">
+        <v>15177</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2383,6 +2445,9 @@
       <c r="Z21" t="n">
         <v>221615</v>
       </c>
+      <c r="AA21" t="n">
+        <v>221637</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2465,6 +2530,9 @@
       <c r="Z22" t="n">
         <v>2608</v>
       </c>
+      <c r="AA22" t="n">
+        <v>2731</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2547,6 +2615,9 @@
       <c r="Z23" t="n">
         <v>2437</v>
       </c>
+      <c r="AA23" t="n">
+        <v>2478</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2629,6 +2700,9 @@
       <c r="Z24" t="n">
         <v>191</v>
       </c>
+      <c r="AA24" t="n">
+        <v>174</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2711,6 +2785,9 @@
       <c r="Z25" t="n">
         <v>1238</v>
       </c>
+      <c r="AA25" t="n">
+        <v>1259</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2793,6 +2870,9 @@
       <c r="Z26" t="n">
         <v>24414</v>
       </c>
+      <c r="AA26" t="n">
+        <v>23602</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2875,6 +2955,9 @@
       <c r="Z27" t="n">
         <v>4719</v>
       </c>
+      <c r="AA27" t="n">
+        <v>4695</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2957,6 +3040,9 @@
       <c r="Z28" t="n">
         <v>9752</v>
       </c>
+      <c r="AA28" t="n">
+        <v>9275</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3039,6 +3125,9 @@
       <c r="Z29" t="n">
         <v>21354</v>
       </c>
+      <c r="AA29" t="n">
+        <v>21412</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3121,6 +3210,9 @@
       <c r="Z30" t="n">
         <v>450</v>
       </c>
+      <c r="AA30" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3203,6 +3295,9 @@
       <c r="Z31" t="n">
         <v>44150</v>
       </c>
+      <c r="AA31" t="n">
+        <v>44095</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3285,6 +3380,9 @@
       <c r="Z32" t="n">
         <v>25713</v>
       </c>
+      <c r="AA32" t="n">
+        <v>24514</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3367,6 +3465,9 @@
       <c r="Z33" t="n">
         <v>3951</v>
       </c>
+      <c r="AA33" t="n">
+        <v>3742</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3449,6 +3550,9 @@
       <c r="Z34" t="n">
         <v>7321</v>
       </c>
+      <c r="AA34" t="n">
+        <v>7373</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3531,6 +3635,9 @@
       <c r="Z35" t="n">
         <v>40210</v>
       </c>
+      <c r="AA35" t="n">
+        <v>40019</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3612,6 +3719,9 @@
       </c>
       <c r="Z36" t="n">
         <v>29793</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>30236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-13 10:35:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA36"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -748,6 +748,11 @@
           <t>12-10-2020</t>
         </is>
       </c>
+      <c r="AB1" s="9" t="inlineStr">
+        <is>
+          <t>13-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -833,6 +838,9 @@
       <c r="AA2" t="n">
         <v>186</v>
       </c>
+      <c r="AB2" t="n">
+        <v>198</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -918,6 +926,9 @@
       <c r="AA3" t="n">
         <v>46295</v>
       </c>
+      <c r="AB3" t="n">
+        <v>43983</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1003,6 +1014,9 @@
       <c r="AA4" t="n">
         <v>2891</v>
       </c>
+      <c r="AB4" t="n">
+        <v>2940</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1088,6 +1102,9 @@
       <c r="AA5" t="n">
         <v>28385</v>
       </c>
+      <c r="AB5" t="n">
+        <v>28439</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1173,6 +1190,9 @@
       <c r="AA6" t="n">
         <v>11044</v>
       </c>
+      <c r="AB6" t="n">
+        <v>10669</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1258,6 +1278,9 @@
       <c r="AA7" t="n">
         <v>1184</v>
       </c>
+      <c r="AB7" t="n">
+        <v>1170</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1343,6 +1366,9 @@
       <c r="AA8" t="n">
         <v>27348</v>
       </c>
+      <c r="AB8" t="n">
+        <v>27421</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1428,6 +1454,9 @@
       <c r="AA9" t="n">
         <v>102</v>
       </c>
+      <c r="AB9" t="n">
+        <v>102</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1513,6 +1542,9 @@
       <c r="AA10" t="n">
         <v>21701</v>
       </c>
+      <c r="AB10" t="n">
+        <v>20535</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1598,6 +1630,9 @@
       <c r="AA11" t="n">
         <v>4656</v>
       </c>
+      <c r="AB11" t="n">
+        <v>4465</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1683,6 +1718,9 @@
       <c r="AA12" t="n">
         <v>15695</v>
       </c>
+      <c r="AB12" t="n">
+        <v>15414</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1768,6 +1806,9 @@
       <c r="AA13" t="n">
         <v>10573</v>
       </c>
+      <c r="AB13" t="n">
+        <v>10401</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1853,6 +1894,9 @@
       <c r="AA14" t="n">
         <v>2687</v>
       </c>
+      <c r="AB14" t="n">
+        <v>2637</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1938,6 +1982,9 @@
       <c r="AA15" t="n">
         <v>10466</v>
       </c>
+      <c r="AB15" t="n">
+        <v>9992</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2023,6 +2070,9 @@
       <c r="AA16" t="n">
         <v>8167</v>
       </c>
+      <c r="AB16" t="n">
+        <v>7776</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2108,6 +2158,9 @@
       <c r="AA17" t="n">
         <v>120289</v>
       </c>
+      <c r="AB17" t="n">
+        <v>115795</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2193,6 +2246,9 @@
       <c r="AA18" t="n">
         <v>96401</v>
       </c>
+      <c r="AB18" t="n">
+        <v>94473</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2278,6 +2334,9 @@
       <c r="AA19" t="n">
         <v>980</v>
       </c>
+      <c r="AB19" t="n">
+        <v>961</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2363,6 +2422,9 @@
       <c r="AA20" t="n">
         <v>15177</v>
       </c>
+      <c r="AB20" t="n">
+        <v>14932</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2448,6 +2510,9 @@
       <c r="AA21" t="n">
         <v>221637</v>
       </c>
+      <c r="AB21" t="n">
+        <v>212905</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2533,6 +2598,9 @@
       <c r="AA22" t="n">
         <v>2731</v>
       </c>
+      <c r="AB22" t="n">
+        <v>2756</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2618,6 +2686,9 @@
       <c r="AA23" t="n">
         <v>2478</v>
       </c>
+      <c r="AB23" t="n">
+        <v>2434</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2703,6 +2774,9 @@
       <c r="AA24" t="n">
         <v>174</v>
       </c>
+      <c r="AB24" t="n">
+        <v>156</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2788,6 +2862,9 @@
       <c r="AA25" t="n">
         <v>1259</v>
       </c>
+      <c r="AB25" t="n">
+        <v>1409</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2873,6 +2950,9 @@
       <c r="AA26" t="n">
         <v>23602</v>
       </c>
+      <c r="AB26" t="n">
+        <v>23430</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2958,6 +3038,9 @@
       <c r="AA27" t="n">
         <v>4695</v>
       </c>
+      <c r="AB27" t="n">
+        <v>4617</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3043,6 +3126,9 @@
       <c r="AA28" t="n">
         <v>9275</v>
       </c>
+      <c r="AB28" t="n">
+        <v>8576</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3128,6 +3214,9 @@
       <c r="AA29" t="n">
         <v>21412</v>
       </c>
+      <c r="AB29" t="n">
+        <v>21671</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3213,6 +3302,9 @@
       <c r="AA30" t="n">
         <v>384</v>
       </c>
+      <c r="AB30" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3298,6 +3390,9 @@
       <c r="AA31" t="n">
         <v>44095</v>
       </c>
+      <c r="AB31" t="n">
+        <v>43747</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3383,6 +3478,9 @@
       <c r="AA32" t="n">
         <v>24514</v>
       </c>
+      <c r="AB32" t="n">
+        <v>24208</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3468,6 +3566,9 @@
       <c r="AA33" t="n">
         <v>3742</v>
       </c>
+      <c r="AB33" t="n">
+        <v>3738</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3553,6 +3654,9 @@
       <c r="AA34" t="n">
         <v>7373</v>
       </c>
+      <c r="AB34" t="n">
+        <v>6976</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3638,6 +3742,9 @@
       <c r="AA35" t="n">
         <v>40019</v>
       </c>
+      <c r="AB35" t="n">
+        <v>38815</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3722,6 +3829,9 @@
       </c>
       <c r="AA36" t="n">
         <v>30236</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>30604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-14 10:35:08
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -753,6 +753,11 @@
           <t>13-10-2020</t>
         </is>
       </c>
+      <c r="AC1" s="9" t="inlineStr">
+        <is>
+          <t>14-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -841,6 +846,9 @@
       <c r="AB2" t="n">
         <v>198</v>
       </c>
+      <c r="AC2" t="n">
+        <v>199</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -929,6 +937,9 @@
       <c r="AB3" t="n">
         <v>43983</v>
       </c>
+      <c r="AC3" t="n">
+        <v>42855</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1017,6 +1028,9 @@
       <c r="AB4" t="n">
         <v>2940</v>
       </c>
+      <c r="AC4" t="n">
+        <v>2960</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1105,6 +1119,9 @@
       <c r="AB5" t="n">
         <v>28439</v>
       </c>
+      <c r="AC5" t="n">
+        <v>28897</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1193,6 +1210,9 @@
       <c r="AB6" t="n">
         <v>10669</v>
       </c>
+      <c r="AC6" t="n">
+        <v>10835</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1281,6 +1301,9 @@
       <c r="AB7" t="n">
         <v>1170</v>
       </c>
+      <c r="AC7" t="n">
+        <v>1127</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1369,6 +1392,9 @@
       <c r="AB8" t="n">
         <v>27421</v>
       </c>
+      <c r="AC8" t="n">
+        <v>27208</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1457,6 +1483,9 @@
       <c r="AB9" t="n">
         <v>102</v>
       </c>
+      <c r="AC9" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1545,6 +1574,9 @@
       <c r="AB10" t="n">
         <v>20535</v>
       </c>
+      <c r="AC10" t="n">
+        <v>21490</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1633,6 +1665,9 @@
       <c r="AB11" t="n">
         <v>4465</v>
       </c>
+      <c r="AC11" t="n">
+        <v>4316</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1721,6 +1756,9 @@
       <c r="AB12" t="n">
         <v>15414</v>
       </c>
+      <c r="AC12" t="n">
+        <v>15187</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1809,6 +1847,9 @@
       <c r="AB13" t="n">
         <v>10401</v>
       </c>
+      <c r="AC13" t="n">
+        <v>10319</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1897,6 +1938,9 @@
       <c r="AB14" t="n">
         <v>2637</v>
       </c>
+      <c r="AC14" t="n">
+        <v>2507</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1985,6 +2029,9 @@
       <c r="AB15" t="n">
         <v>9992</v>
       </c>
+      <c r="AC15" t="n">
+        <v>9866</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2073,6 +2120,9 @@
       <c r="AB16" t="n">
         <v>7776</v>
       </c>
+      <c r="AC16" t="n">
+        <v>7617</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2161,6 +2211,9 @@
       <c r="AB17" t="n">
         <v>115795</v>
       </c>
+      <c r="AC17" t="n">
+        <v>113478</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2249,6 +2302,9 @@
       <c r="AB18" t="n">
         <v>94473</v>
       </c>
+      <c r="AC18" t="n">
+        <v>95493</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2337,6 +2393,9 @@
       <c r="AB19" t="n">
         <v>961</v>
       </c>
+      <c r="AC19" t="n">
+        <v>969</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2425,6 +2484,9 @@
       <c r="AB20" t="n">
         <v>14932</v>
       </c>
+      <c r="AC20" t="n">
+        <v>14661</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2513,6 +2575,9 @@
       <c r="AB21" t="n">
         <v>212905</v>
       </c>
+      <c r="AC21" t="n">
+        <v>205884</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2601,6 +2666,9 @@
       <c r="AB22" t="n">
         <v>2756</v>
       </c>
+      <c r="AC22" t="n">
+        <v>2867</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2689,6 +2757,9 @@
       <c r="AB23" t="n">
         <v>2434</v>
       </c>
+      <c r="AC23" t="n">
+        <v>2367</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2777,6 +2848,9 @@
       <c r="AB24" t="n">
         <v>156</v>
       </c>
+      <c r="AC24" t="n">
+        <v>119</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2865,6 +2939,9 @@
       <c r="AB25" t="n">
         <v>1409</v>
       </c>
+      <c r="AC25" t="n">
+        <v>1513</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2953,6 +3030,9 @@
       <c r="AB26" t="n">
         <v>23430</v>
       </c>
+      <c r="AC26" t="n">
+        <v>22892</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3041,6 +3121,9 @@
       <c r="AB27" t="n">
         <v>4617</v>
       </c>
+      <c r="AC27" t="n">
+        <v>4572</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3129,6 +3212,9 @@
       <c r="AB28" t="n">
         <v>8576</v>
       </c>
+      <c r="AC28" t="n">
+        <v>8212</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3217,6 +3303,9 @@
       <c r="AB29" t="n">
         <v>21671</v>
       </c>
+      <c r="AC29" t="n">
+        <v>21924</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3305,6 +3394,9 @@
       <c r="AB30" t="n">
         <v>384</v>
       </c>
+      <c r="AC30" t="n">
+        <v>344</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3393,6 +3485,9 @@
       <c r="AB31" t="n">
         <v>43747</v>
       </c>
+      <c r="AC31" t="n">
+        <v>43239</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3481,6 +3576,9 @@
       <c r="AB32" t="n">
         <v>24208</v>
       </c>
+      <c r="AC32" t="n">
+        <v>23728</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3569,6 +3667,9 @@
       <c r="AB33" t="n">
         <v>3738</v>
       </c>
+      <c r="AC33" t="n">
+        <v>3500</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3657,6 +3758,9 @@
       <c r="AB34" t="n">
         <v>6976</v>
       </c>
+      <c r="AC34" t="n">
+        <v>6576</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3745,6 +3849,9 @@
       <c r="AB35" t="n">
         <v>38815</v>
       </c>
+      <c r="AC35" t="n">
+        <v>38082</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3832,6 +3939,9 @@
       </c>
       <c r="AB36" t="n">
         <v>30604</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>30988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-15 10:35:09
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC36"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -758,6 +758,11 @@
           <t>14-10-2020</t>
         </is>
       </c>
+      <c r="AD1" s="9" t="inlineStr">
+        <is>
+          <t>15-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -849,6 +854,9 @@
       <c r="AC2" t="n">
         <v>199</v>
       </c>
+      <c r="AD2" t="n">
+        <v>195</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -940,6 +948,9 @@
       <c r="AC3" t="n">
         <v>42855</v>
       </c>
+      <c r="AD3" t="n">
+        <v>41669</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1031,6 +1042,9 @@
       <c r="AC4" t="n">
         <v>2960</v>
       </c>
+      <c r="AD4" t="n">
+        <v>3045</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1122,6 +1136,9 @@
       <c r="AC5" t="n">
         <v>28897</v>
       </c>
+      <c r="AD5" t="n">
+        <v>29307</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1213,6 +1230,9 @@
       <c r="AC6" t="n">
         <v>10835</v>
       </c>
+      <c r="AD6" t="n">
+        <v>10756</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1304,6 +1324,9 @@
       <c r="AC7" t="n">
         <v>1127</v>
       </c>
+      <c r="AD7" t="n">
+        <v>1085</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1395,6 +1418,9 @@
       <c r="AC8" t="n">
         <v>27208</v>
       </c>
+      <c r="AD8" t="n">
+        <v>27809</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1486,6 +1512,9 @@
       <c r="AC9" t="n">
         <v>85</v>
       </c>
+      <c r="AD9" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1577,6 +1606,9 @@
       <c r="AC10" t="n">
         <v>21490</v>
       </c>
+      <c r="AD10" t="n">
+        <v>21903</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1668,6 +1700,9 @@
       <c r="AC11" t="n">
         <v>4316</v>
       </c>
+      <c r="AD11" t="n">
+        <v>4188</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1759,6 +1794,9 @@
       <c r="AC12" t="n">
         <v>15187</v>
       </c>
+      <c r="AD12" t="n">
+        <v>14937</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1850,6 +1888,9 @@
       <c r="AC13" t="n">
         <v>10319</v>
       </c>
+      <c r="AD13" t="n">
+        <v>10187</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1941,6 +1982,9 @@
       <c r="AC14" t="n">
         <v>2507</v>
       </c>
+      <c r="AD14" t="n">
+        <v>2520</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2032,6 +2076,9 @@
       <c r="AC15" t="n">
         <v>9866</v>
       </c>
+      <c r="AD15" t="n">
+        <v>9739</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2123,6 +2170,9 @@
       <c r="AC16" t="n">
         <v>7617</v>
       </c>
+      <c r="AD16" t="n">
+        <v>7191</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2214,6 +2264,9 @@
       <c r="AC17" t="n">
         <v>113478</v>
       </c>
+      <c r="AD17" t="n">
+        <v>114006</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2305,6 +2358,9 @@
       <c r="AC18" t="n">
         <v>95493</v>
       </c>
+      <c r="AD18" t="n">
+        <v>93925</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2396,6 +2452,9 @@
       <c r="AC19" t="n">
         <v>969</v>
       </c>
+      <c r="AD19" t="n">
+        <v>979</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2487,6 +2546,9 @@
       <c r="AC20" t="n">
         <v>14661</v>
       </c>
+      <c r="AD20" t="n">
+        <v>14432</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2578,6 +2640,9 @@
       <c r="AC21" t="n">
         <v>205884</v>
       </c>
+      <c r="AD21" t="n">
+        <v>196761</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2669,6 +2734,9 @@
       <c r="AC22" t="n">
         <v>2867</v>
       </c>
+      <c r="AD22" t="n">
+        <v>3076</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2760,6 +2828,9 @@
       <c r="AC23" t="n">
         <v>2367</v>
       </c>
+      <c r="AD23" t="n">
+        <v>2339</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2851,6 +2922,9 @@
       <c r="AC24" t="n">
         <v>119</v>
       </c>
+      <c r="AD24" t="n">
+        <v>112</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2942,6 +3016,9 @@
       <c r="AC25" t="n">
         <v>1513</v>
       </c>
+      <c r="AD25" t="n">
+        <v>1478</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3033,6 +3110,9 @@
       <c r="AC26" t="n">
         <v>22892</v>
       </c>
+      <c r="AD26" t="n">
+        <v>22716</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3124,6 +3204,9 @@
       <c r="AC27" t="n">
         <v>4572</v>
       </c>
+      <c r="AD27" t="n">
+        <v>4525</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3215,6 +3298,9 @@
       <c r="AC28" t="n">
         <v>8212</v>
       </c>
+      <c r="AD28" t="n">
+        <v>7760</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3306,6 +3392,9 @@
       <c r="AC29" t="n">
         <v>21924</v>
       </c>
+      <c r="AD29" t="n">
+        <v>21711</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3397,6 +3486,9 @@
       <c r="AC30" t="n">
         <v>344</v>
       </c>
+      <c r="AD30" t="n">
+        <v>325</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3488,6 +3580,9 @@
       <c r="AC31" t="n">
         <v>43239</v>
       </c>
+      <c r="AD31" t="n">
+        <v>42566</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3579,6 +3674,9 @@
       <c r="AC32" t="n">
         <v>23728</v>
       </c>
+      <c r="AD32" t="n">
+        <v>23203</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3670,6 +3768,9 @@
       <c r="AC33" t="n">
         <v>3500</v>
       </c>
+      <c r="AD33" t="n">
+        <v>3318</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3761,6 +3862,9 @@
       <c r="AC34" t="n">
         <v>6576</v>
       </c>
+      <c r="AD34" t="n">
+        <v>6145</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3852,6 +3956,9 @@
       <c r="AC35" t="n">
         <v>38082</v>
       </c>
+      <c r="AD35" t="n">
+        <v>36898</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3942,6 +4049,9 @@
       </c>
       <c r="AC36" t="n">
         <v>30988</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>31505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files are pushed at time 2020-10-16 10:35:06
</commit_message>
<xml_diff>
--- a/excelfiles/active_cases.xlsx
+++ b/excelfiles/active_cases.xlsx
@@ -604,7 +604,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD36"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
@@ -763,6 +763,11 @@
           <t>15-10-2020</t>
         </is>
       </c>
+      <c r="AE1" s="9" t="inlineStr">
+        <is>
+          <t>16-10-2020</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -857,6 +862,9 @@
       <c r="AD2" t="n">
         <v>195</v>
       </c>
+      <c r="AE2" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -951,6 +959,9 @@
       <c r="AD3" t="n">
         <v>41669</v>
       </c>
+      <c r="AE3" t="n">
+        <v>40047</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1045,6 +1056,9 @@
       <c r="AD4" t="n">
         <v>3045</v>
       </c>
+      <c r="AE4" t="n">
+        <v>3052</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1139,6 +1153,9 @@
       <c r="AD5" t="n">
         <v>29307</v>
       </c>
+      <c r="AE5" t="n">
+        <v>28804</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1233,6 +1250,9 @@
       <c r="AD6" t="n">
         <v>10756</v>
       </c>
+      <c r="AE6" t="n">
+        <v>11038</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1327,6 +1347,9 @@
       <c r="AD7" t="n">
         <v>1085</v>
       </c>
+      <c r="AE7" t="n">
+        <v>1044</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1421,6 +1444,9 @@
       <c r="AD8" t="n">
         <v>27809</v>
       </c>
+      <c r="AE8" t="n">
+        <v>28187</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1515,6 +1541,9 @@
       <c r="AD9" t="n">
         <v>79</v>
       </c>
+      <c r="AE9" t="n">
+        <v>71</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1609,6 +1638,9 @@
       <c r="AD10" t="n">
         <v>21903</v>
       </c>
+      <c r="AE10" t="n">
+        <v>22605</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1703,6 +1735,9 @@
       <c r="AD11" t="n">
         <v>4188</v>
       </c>
+      <c r="AE11" t="n">
+        <v>4084</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1797,6 +1832,9 @@
       <c r="AD12" t="n">
         <v>14937</v>
       </c>
+      <c r="AE12" t="n">
+        <v>14782</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1891,6 +1929,9 @@
       <c r="AD13" t="n">
         <v>10187</v>
       </c>
+      <c r="AE13" t="n">
+        <v>10364</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1985,6 +2026,9 @@
       <c r="AD14" t="n">
         <v>2520</v>
       </c>
+      <c r="AE14" t="n">
+        <v>2654</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2079,6 +2123,9 @@
       <c r="AD15" t="n">
         <v>9739</v>
       </c>
+      <c r="AE15" t="n">
+        <v>9058</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2173,6 +2220,9 @@
       <c r="AD16" t="n">
         <v>7191</v>
       </c>
+      <c r="AE16" t="n">
+        <v>6892</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2267,6 +2317,9 @@
       <c r="AD17" t="n">
         <v>114006</v>
       </c>
+      <c r="AE17" t="n">
+        <v>113557</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2361,6 +2414,9 @@
       <c r="AD18" t="n">
         <v>93925</v>
       </c>
+      <c r="AE18" t="n">
+        <v>94609</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2455,6 +2511,9 @@
       <c r="AD19" t="n">
         <v>979</v>
       </c>
+      <c r="AE19" t="n">
+        <v>1018</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2549,6 +2608,9 @@
       <c r="AD20" t="n">
         <v>14432</v>
       </c>
+      <c r="AE20" t="n">
+        <v>14157</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2643,6 +2705,9 @@
       <c r="AD21" t="n">
         <v>196761</v>
       </c>
+      <c r="AE21" t="n">
+        <v>192936</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2737,6 +2802,9 @@
       <c r="AD22" t="n">
         <v>3076</v>
       </c>
+      <c r="AE22" t="n">
+        <v>3193</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2831,6 +2899,9 @@
       <c r="AD23" t="n">
         <v>2339</v>
       </c>
+      <c r="AE23" t="n">
+        <v>2445</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2925,6 +2996,9 @@
       <c r="AD24" t="n">
         <v>112</v>
       </c>
+      <c r="AE24" t="n">
+        <v>108</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3019,6 +3093,9 @@
       <c r="AD25" t="n">
         <v>1478</v>
       </c>
+      <c r="AE25" t="n">
+        <v>1453</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3113,6 +3190,9 @@
       <c r="AD26" t="n">
         <v>22716</v>
       </c>
+      <c r="AE26" t="n">
+        <v>22387</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3207,6 +3287,9 @@
       <c r="AD27" t="n">
         <v>4525</v>
       </c>
+      <c r="AE27" t="n">
+        <v>4551</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3301,6 +3384,9 @@
       <c r="AD28" t="n">
         <v>7760</v>
       </c>
+      <c r="AE28" t="n">
+        <v>7090</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3395,6 +3481,9 @@
       <c r="AD29" t="n">
         <v>21711</v>
       </c>
+      <c r="AE29" t="n">
+        <v>21587</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3489,6 +3578,9 @@
       <c r="AD30" t="n">
         <v>325</v>
       </c>
+      <c r="AE30" t="n">
+        <v>312</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3583,6 +3675,9 @@
       <c r="AD31" t="n">
         <v>42566</v>
       </c>
+      <c r="AE31" t="n">
+        <v>41872</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3677,6 +3772,9 @@
       <c r="AD32" t="n">
         <v>23203</v>
       </c>
+      <c r="AE32" t="n">
+        <v>23315</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3771,6 +3869,9 @@
       <c r="AD33" t="n">
         <v>3318</v>
       </c>
+      <c r="AE33" t="n">
+        <v>3105</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3865,6 +3966,9 @@
       <c r="AD34" t="n">
         <v>6145</v>
       </c>
+      <c r="AE34" t="n">
+        <v>5682</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3959,6 +4063,9 @@
       <c r="AD35" t="n">
         <v>36898</v>
       </c>
+      <c r="AE35" t="n">
+        <v>36295</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4052,6 +4159,9 @@
       </c>
       <c r="AD36" t="n">
         <v>31505</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>31984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>